<commit_message>
improvements to invoice printing
</commit_message>
<xml_diff>
--- a/Design.xlsx
+++ b/Design.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="299">
   <si>
     <t>sales_person</t>
   </si>
@@ -798,12 +798,6 @@
     <t>Summary Page</t>
   </si>
   <si>
-    <t>Summary Page Calculation - Deepak</t>
-  </si>
-  <si>
-    <t>Payment Type : Cash / Card - as dropdown - Deepak</t>
-  </si>
-  <si>
     <t xml:space="preserve">When Summary is clicked, Need to print the invoice </t>
   </si>
   <si>
@@ -849,13 +843,82 @@
     <t>Cart Item able to edit</t>
   </si>
   <si>
-    <t>Make coloured Grid</t>
-  </si>
-  <si>
     <t>Able to print invoice, full company details as header in pdf</t>
   </si>
   <si>
     <t>Able to create apk file - Lakshmy</t>
+  </si>
+  <si>
+    <t>Able to edit Invoice</t>
+  </si>
+  <si>
+    <t>Excel Download</t>
+  </si>
+  <si>
+    <t>Customer Vat No</t>
+  </si>
+  <si>
+    <t>Discount for each item</t>
+  </si>
+  <si>
+    <t>Category Master</t>
+  </si>
+  <si>
+    <t>Brand Master</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Able to Add/Delete/Update </t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Search in Category, Product</t>
+  </si>
+  <si>
+    <t>Ability to reduce clicks</t>
+  </si>
+  <si>
+    <t>Ability to sink image from web server to mobile app</t>
+  </si>
+  <si>
+    <t>JSON</t>
+  </si>
+  <si>
+    <t>Mobile App</t>
+  </si>
+  <si>
+    <t>Rest Service</t>
+  </si>
+  <si>
+    <t>Printer</t>
+  </si>
+  <si>
+    <t>Option 1</t>
+  </si>
+  <si>
+    <t>Processing</t>
+  </si>
+  <si>
+    <t>JSON - HTML - PDF- Print</t>
+  </si>
+  <si>
+    <t>Physical printing</t>
+  </si>
+  <si>
+    <t>Option 2</t>
+  </si>
+  <si>
+    <t>HTML - PDF- Print</t>
+  </si>
+  <si>
+    <t>Make coloured Grid - in future</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summary Page Calculation </t>
+  </si>
+  <si>
+    <t>Payment Type : Cash / Card - as dropdown</t>
   </si>
 </sst>
 </file>
@@ -1474,6 +1537,9 @@
     <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1504,9 +1570,6 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2470,10 +2533,10 @@
       <c r="D30" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E30" s="165"/>
-      <c r="F30" s="165"/>
-      <c r="G30" s="165"/>
-      <c r="H30" s="166"/>
+      <c r="E30" s="168"/>
+      <c r="F30" s="168"/>
+      <c r="G30" s="168"/>
+      <c r="H30" s="169"/>
     </row>
     <row r="31" spans="2:10">
       <c r="B31" s="3"/>
@@ -2958,8 +3021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R83"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2994,28 +3057,28 @@
     </row>
     <row r="3" spans="1:9">
       <c r="B3" s="48"/>
-      <c r="C3" s="167" t="s">
+      <c r="C3" s="170" t="s">
         <v>152</v>
       </c>
-      <c r="D3" s="167"/>
+      <c r="D3" s="170"/>
       <c r="E3" s="147"/>
       <c r="F3" s="51"/>
     </row>
     <row r="4" spans="1:9">
       <c r="B4" s="48"/>
-      <c r="C4" s="167" t="s">
+      <c r="C4" s="170" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="167"/>
+      <c r="D4" s="170"/>
       <c r="E4" s="147"/>
       <c r="F4" s="51"/>
     </row>
     <row r="5" spans="1:9">
       <c r="B5" s="48"/>
-      <c r="C5" s="167" t="s">
+      <c r="C5" s="170" t="s">
         <v>153</v>
       </c>
-      <c r="D5" s="167"/>
+      <c r="D5" s="170"/>
       <c r="E5" s="147"/>
       <c r="F5" s="51"/>
     </row>
@@ -4348,8 +4411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C5:I55"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4367,26 +4430,26 @@
     </row>
     <row r="6" spans="3:9">
       <c r="C6" s="48"/>
-      <c r="D6" s="167" t="s">
+      <c r="D6" s="170" t="s">
         <v>152</v>
       </c>
-      <c r="E6" s="167"/>
+      <c r="E6" s="170"/>
       <c r="F6" s="51"/>
     </row>
     <row r="7" spans="3:9">
       <c r="C7" s="48"/>
-      <c r="D7" s="167" t="s">
+      <c r="D7" s="170" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="167"/>
+      <c r="E7" s="170"/>
       <c r="F7" s="51"/>
     </row>
     <row r="8" spans="3:9">
       <c r="C8" s="48"/>
-      <c r="D8" s="167" t="s">
+      <c r="D8" s="170" t="s">
         <v>153</v>
       </c>
-      <c r="E8" s="167"/>
+      <c r="E8" s="170"/>
       <c r="F8" s="51"/>
     </row>
     <row r="9" spans="3:9">
@@ -4431,10 +4494,10 @@
     </row>
     <row r="15" spans="3:9">
       <c r="C15" s="48"/>
-      <c r="D15" s="168" t="s">
+      <c r="D15" s="171" t="s">
         <v>165</v>
       </c>
-      <c r="E15" s="169"/>
+      <c r="E15" s="172"/>
       <c r="F15" s="51"/>
       <c r="H15" t="s">
         <v>33</v>
@@ -4461,14 +4524,14 @@
       </c>
     </row>
     <row r="19" spans="3:9">
-      <c r="C19" s="172" t="s">
+      <c r="C19" s="175" t="s">
         <v>235</v>
       </c>
-      <c r="D19" s="173"/>
-      <c r="E19" s="170" t="s">
+      <c r="D19" s="176"/>
+      <c r="E19" s="173" t="s">
         <v>166</v>
       </c>
-      <c r="F19" s="174"/>
+      <c r="F19" s="177"/>
       <c r="H19" t="s">
         <v>32</v>
       </c>
@@ -4585,14 +4648,14 @@
       </c>
     </row>
     <row r="36" spans="3:6">
-      <c r="C36" s="170" t="s">
+      <c r="C36" s="173" t="s">
         <v>234</v>
       </c>
-      <c r="D36" s="171"/>
-      <c r="E36" s="172" t="s">
+      <c r="D36" s="174"/>
+      <c r="E36" s="175" t="s">
         <v>166</v>
       </c>
-      <c r="F36" s="173"/>
+      <c r="F36" s="176"/>
     </row>
     <row r="37" spans="3:6">
       <c r="C37" s="121"/>
@@ -4720,10 +4783,10 @@
     </row>
     <row r="53" spans="3:9">
       <c r="C53" s="121"/>
-      <c r="D53" s="168" t="s">
+      <c r="D53" s="171" t="s">
         <v>162</v>
       </c>
-      <c r="E53" s="169"/>
+      <c r="E53" s="172"/>
       <c r="F53" s="123"/>
       <c r="H53" t="s">
         <v>33</v>
@@ -4955,10 +5018,10 @@
     </row>
     <row r="23" spans="3:6">
       <c r="C23" s="48"/>
-      <c r="D23" s="168" t="s">
+      <c r="D23" s="171" t="s">
         <v>156</v>
       </c>
-      <c r="E23" s="169"/>
+      <c r="E23" s="172"/>
       <c r="F23" s="51"/>
     </row>
     <row r="24" spans="3:6">
@@ -5010,7 +5073,7 @@
   <dimension ref="A2:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5021,9 +5084,9 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3">
-      <c r="A2" s="176"/>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
+      <c r="A2" s="166"/>
+      <c r="B2" s="166"/>
+      <c r="C2" s="166"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
@@ -5041,13 +5104,13 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="176"/>
-      <c r="B7" s="176"/>
-      <c r="C7" s="176"/>
+      <c r="A7" s="166"/>
+      <c r="B7" s="166"/>
+      <c r="C7" s="166"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
@@ -5073,7 +5136,7 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -5083,10 +5146,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5096,9 +5159,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="176"/>
-      <c r="B1" s="176"/>
-      <c r="C1" s="176"/>
+      <c r="A1" s="166"/>
+      <c r="B1" s="166"/>
+      <c r="C1" s="166"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
@@ -5121,125 +5184,163 @@
         <v>245</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="177"/>
-      <c r="B11" s="177"/>
-      <c r="C11" s="177"/>
+    <row r="7" spans="1:3">
+      <c r="A7" s="167"/>
+      <c r="B7" s="167"/>
+      <c r="C7" s="167"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>263</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" t="s">
+      <c r="A12" s="166"/>
+      <c r="B12" s="166"/>
+      <c r="C12" s="166"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="166"/>
+      <c r="B25" s="166"/>
+      <c r="C25" s="166"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>260</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>279</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>280</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="166"/>
+      <c r="B39" s="166"/>
+      <c r="C39" s="166"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>264</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
         <v>265</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
+    </row>
+    <row r="41" spans="1:3">
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="176"/>
-      <c r="B19" s="176"/>
-      <c r="C19" s="176"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>141</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="B22">
-        <v>3</v>
-      </c>
-      <c r="C22" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="B23">
-        <v>4</v>
-      </c>
-      <c r="C23" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="B24">
-        <v>5</v>
-      </c>
-      <c r="C24" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="B25">
-        <v>6</v>
-      </c>
-      <c r="C25" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="176"/>
-      <c r="B32" s="176"/>
-      <c r="C32" s="176"/>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>262</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="176"/>
-      <c r="B38" s="176"/>
-      <c r="C38" s="176"/>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
+    <row r="46" spans="1:3">
+      <c r="A46" s="165" t="s">
         <v>266</v>
       </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="B46" s="165"/>
+      <c r="C46" s="165" t="s">
         <v>267</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="175" t="s">
-        <v>268</v>
-      </c>
-      <c r="B45" s="175"/>
-      <c r="C45" s="175" t="s">
-        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -5250,23 +5351,27 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:C12"/>
+  <dimension ref="A2:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3">
-      <c r="A2" s="176"/>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-    </row>
-    <row r="3" spans="1:3">
+    <row r="2" spans="1:11">
+      <c r="A2" s="166"/>
+      <c r="B2" s="166"/>
+      <c r="C2" s="166"/>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>257</v>
       </c>
@@ -5274,63 +5379,150 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="176"/>
-      <c r="B8" s="176"/>
-      <c r="C8" s="176"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>273</v>
-      </c>
-      <c r="B9">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="166"/>
+      <c r="B9" s="166"/>
+      <c r="C9" s="166"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>271</v>
+      </c>
+      <c r="B10">
         <v>1</v>
       </c>
-      <c r="C9" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="176"/>
-      <c r="B11" s="176"/>
-      <c r="C11" s="176"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
+      <c r="C10" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>278</v>
+      </c>
+      <c r="G11" s="166"/>
+      <c r="H11" s="166" t="s">
+        <v>287</v>
+      </c>
+      <c r="I11" s="166" t="s">
+        <v>291</v>
+      </c>
+      <c r="J11" s="166" t="s">
+        <v>288</v>
+      </c>
+      <c r="K11" s="166" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="166"/>
+      <c r="B13" s="166"/>
+      <c r="C13" s="166"/>
+      <c r="G13" t="s">
+        <v>290</v>
+      </c>
+      <c r="H13" t="s">
+        <v>286</v>
+      </c>
+      <c r="I13" t="s">
+        <v>292</v>
+      </c>
+      <c r="K13" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
         <v>160</v>
       </c>
-      <c r="B12">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="G15" t="s">
+        <v>294</v>
+      </c>
+      <c r="H15" t="s">
+        <v>286</v>
+      </c>
+      <c r="J15" t="s">
+        <v>295</v>
+      </c>
+      <c r="K15" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="166"/>
+      <c r="B17" s="166"/>
+      <c r="C17" s="166"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>282</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="B19">
         <v>2</v>
       </c>
-      <c r="C12" t="s">
-        <v>274</v>
+      <c r="C19" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>